<commit_message>
Bcora 13 Abril Inicio
</commit_message>
<xml_diff>
--- a/Bitacoras/1.incio 13 marzo/BITACORA ETAPA PRODUCTIVA.xlsx
+++ b/Bitacoras/1.incio 13 marzo/BITACORA ETAPA PRODUCTIVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferney.ruiz\Documents\GitHub\Files-Practice\Bitacoras\1.incio 13 marzo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9AF65FFC-A614-42D6-AA06-1BFC348363C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9ACCDC8D-CC93-43F7-A92A-50C8909960BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Bogotá D.C</t>
-  </si>
-  <si>
-    <t>Josemar David Sierra Ramirez</t>
   </si>
   <si>
     <t>jsierra@lisim.com</t>
@@ -282,9 +279,6 @@
     </r>
   </si>
   <si>
-    <t>Ingeniero Proyecto Senior</t>
-  </si>
-  <si>
     <t>Funciones, procedimientos, tareas especificas del cargo,captura de horas, incluir procedimientos del SIG.</t>
   </si>
   <si>
@@ -301,7 +295,13 @@
     <t>Cargar datos de un archivo plano (txt) a una tabla SQL y de SQL a (txt) por medio de una ETL con Visual Studio</t>
   </si>
   <si>
-    <t>Business Intelligence</t>
+    <t>Miller Ivan Saavedra Forero</t>
+  </si>
+  <si>
+    <t>Lider Business Integillence</t>
+  </si>
+  <si>
+    <t>Analytics</t>
   </si>
 </sst>
 </file>
@@ -860,15 +860,229 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -879,21 +1093,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -927,9 +1126,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -938,202 +1134,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:N38"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31:V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1580,138 +1580,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="94"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="82" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="84"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
+      <c r="V1" s="120"/>
+      <c r="W1" s="121"/>
       <c r="X1" s="3"/>
     </row>
     <row r="2" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="85" t="s">
+      <c r="B2" s="103"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="87"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123"/>
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="124"/>
       <c r="X2" s="3"/>
     </row>
     <row r="3" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="88" t="s">
+      <c r="B3" s="103"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="90"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="127"/>
       <c r="X3" s="3"/>
     </row>
     <row r="4" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="88" t="s">
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="90"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="126"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="126"/>
+      <c r="Q4" s="126"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="126"/>
+      <c r="U4" s="126"/>
+      <c r="V4" s="126"/>
+      <c r="W4" s="127"/>
       <c r="X4" s="3"/>
     </row>
     <row r="5" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="91" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="92"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="93"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="129"/>
+      <c r="Q5" s="129"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="129"/>
+      <c r="T5" s="129"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="129"/>
+      <c r="W5" s="130"/>
       <c r="X5" s="3"/>
     </row>
     <row r="6" spans="1:24" s="4" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,30 +1740,30 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="97"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="97"/>
+      <c r="V7" s="97"/>
+      <c r="W7" s="97"/>
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" s="27" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1824,24 +1824,24 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="34"/>
-      <c r="E10" s="71" t="s">
+      <c r="E10" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="70" t="s">
+      <c r="F10" s="137"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="137"/>
+      <c r="L10" s="137"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
+      <c r="O10" s="138"/>
+      <c r="P10" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
+      <c r="Q10" s="135"/>
+      <c r="R10" s="135"/>
       <c r="S10" s="30" t="s">
         <v>11</v>
       </c>
@@ -1873,9 +1873,9 @@
       <c r="M11" s="6"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="70"/>
+      <c r="P11" s="135"/>
+      <c r="Q11" s="135"/>
+      <c r="R11" s="135"/>
       <c r="S11" s="38"/>
       <c r="T11" s="52"/>
       <c r="U11" s="52"/>
@@ -1889,26 +1889,26 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="79">
+      <c r="E12" s="143">
         <v>1056592950</v>
       </c>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
+      <c r="F12" s="144"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="144"/>
+      <c r="J12" s="145"/>
       <c r="K12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="140"/>
+      <c r="O12" s="141"/>
+      <c r="P12" s="135"/>
+      <c r="Q12" s="135"/>
+      <c r="R12" s="135"/>
       <c r="S12" s="30" t="s">
         <v>12</v>
       </c>
@@ -1955,19 +1955,19 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="78" t="s">
+      <c r="E14" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="63" t="s">
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="106"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="63"/>
-      <c r="M14" s="64"/>
+      <c r="L14" s="133"/>
+      <c r="M14" s="134"/>
       <c r="N14" s="53">
         <v>27</v>
       </c>
@@ -1977,11 +1977,11 @@
       <c r="P14" s="53">
         <v>2018</v>
       </c>
-      <c r="Q14" s="77" t="s">
+      <c r="Q14" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="63"/>
-      <c r="S14" s="64"/>
+      <c r="R14" s="133"/>
+      <c r="S14" s="134"/>
       <c r="T14" s="51">
         <v>27</v>
       </c>
@@ -2025,30 +2025,30 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="99" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="100"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="100"/>
-      <c r="I16" s="100"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="100"/>
-      <c r="L16" s="100"/>
-      <c r="M16" s="100"/>
-      <c r="N16" s="100"/>
-      <c r="O16" s="101"/>
+      <c r="E16" s="111" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="112"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="112"/>
+      <c r="O16" s="113"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="25" t="s">
         <v>4</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
-      <c r="T16" s="102">
+      <c r="T16" s="114">
         <v>1193307</v>
       </c>
-      <c r="U16" s="102"/>
-      <c r="V16" s="102"/>
+      <c r="U16" s="114"/>
+      <c r="V16" s="114"/>
       <c r="W16" s="11"/>
     </row>
     <row r="17" spans="1:24" s="2" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.25">
@@ -2083,32 +2083,32 @@
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
-      <c r="E18" s="103">
+      <c r="E18" s="72">
         <v>3002876907</v>
       </c>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="128" t="s">
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="129"/>
-      <c r="J18" s="124"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="68" t="s">
+      <c r="I18" s="80"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="127"/>
-      <c r="Q18" s="103" t="s">
+      <c r="N18" s="77"/>
+      <c r="O18" s="77"/>
+      <c r="P18" s="78"/>
+      <c r="Q18" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="R18" s="103"/>
-      <c r="S18" s="103"/>
-      <c r="T18" s="103"/>
-      <c r="U18" s="103"/>
-      <c r="V18" s="103"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="72"/>
+      <c r="T18" s="72"/>
+      <c r="U18" s="72"/>
+      <c r="V18" s="72"/>
       <c r="W18" s="11"/>
     </row>
     <row r="19" spans="1:24" s="2" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2187,30 +2187,30 @@
       <c r="W21" s="31"/>
     </row>
     <row r="22" spans="1:24" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="97"/>
+      <c r="I22" s="97"/>
+      <c r="J22" s="97"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="97"/>
+      <c r="S22" s="97"/>
+      <c r="T22" s="97"/>
+      <c r="U22" s="97"/>
+      <c r="V22" s="97"/>
+      <c r="W22" s="97"/>
       <c r="X22" s="2"/>
     </row>
     <row r="23" spans="1:24" s="4" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2272,29 +2272,29 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="65" t="s">
+      <c r="F25" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="66"/>
-      <c r="L25" s="66"/>
-      <c r="M25" s="66"/>
-      <c r="N25" s="66"/>
-      <c r="O25" s="66"/>
-      <c r="P25" s="67"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="106"/>
+      <c r="K25" s="106"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="107"/>
       <c r="Q25" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="R25" s="65" t="s">
+      <c r="R25" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="S25" s="66"/>
-      <c r="T25" s="66"/>
-      <c r="U25" s="66"/>
-      <c r="V25" s="67"/>
+      <c r="S25" s="106"/>
+      <c r="T25" s="106"/>
+      <c r="U25" s="106"/>
+      <c r="V25" s="107"/>
       <c r="W25" s="12"/>
     </row>
     <row r="26" spans="1:24" s="2" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.25">
@@ -2328,35 +2328,35 @@
         <v>19</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="65" t="s">
+      <c r="D27" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="67"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="107"/>
       <c r="L27" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="103" t="s">
+      <c r="M27" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="N27" s="103"/>
-      <c r="O27" s="103"/>
-      <c r="P27" s="103"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
       <c r="Q27" s="48" t="s">
         <v>21</v>
       </c>
       <c r="R27" s="49"/>
-      <c r="S27" s="103" t="s">
+      <c r="S27" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="T27" s="103"/>
-      <c r="U27" s="103"/>
-      <c r="V27" s="103"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="72"/>
       <c r="W27" s="22"/>
     </row>
     <row r="28" spans="1:24" s="2" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2390,35 +2390,35 @@
         <v>22</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="68" t="s">
+      <c r="D29" s="105" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="106"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="106"/>
+      <c r="H29" s="106"/>
+      <c r="I29" s="107"/>
+      <c r="J29" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="69"/>
-      <c r="L29" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="M29" s="66"/>
-      <c r="N29" s="66"/>
-      <c r="O29" s="66"/>
-      <c r="P29" s="67"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="M29" s="106"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="106"/>
+      <c r="P29" s="107"/>
       <c r="Q29" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="R29" s="65" t="s">
+      <c r="R29" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="S29" s="66"/>
-      <c r="T29" s="66"/>
-      <c r="U29" s="66"/>
-      <c r="V29" s="67"/>
+      <c r="S29" s="106"/>
+      <c r="T29" s="106"/>
+      <c r="U29" s="106"/>
+      <c r="V29" s="107"/>
       <c r="W29" s="22"/>
     </row>
     <row r="30" spans="1:24" ht="3" customHeight="1" x14ac:dyDescent="0.25">
@@ -2449,36 +2449,36 @@
       <c r="B31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="105" t="s">
+      <c r="C31" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
+      <c r="I31" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="J31" s="106"/>
+      <c r="J31" s="118"/>
       <c r="K31" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="L31" s="104"/>
-      <c r="M31" s="104"/>
-      <c r="N31" s="104"/>
-      <c r="O31" s="104"/>
-      <c r="P31" s="104"/>
+      <c r="L31" s="116"/>
+      <c r="M31" s="116"/>
+      <c r="N31" s="116"/>
+      <c r="O31" s="116"/>
+      <c r="P31" s="116"/>
       <c r="Q31" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="R31" s="96">
-        <v>3168755152</v>
-      </c>
-      <c r="S31" s="97"/>
-      <c r="T31" s="97"/>
-      <c r="U31" s="97"/>
-      <c r="V31" s="98"/>
+      <c r="R31" s="108">
+        <v>3219374373</v>
+      </c>
+      <c r="S31" s="109"/>
+      <c r="T31" s="109"/>
+      <c r="U31" s="109"/>
+      <c r="V31" s="110"/>
       <c r="W31" s="43"/>
     </row>
     <row r="32" spans="1:24" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2531,30 +2531,30 @@
       <c r="W33" s="31"/>
     </row>
     <row r="34" spans="1:24" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="58"/>
-      <c r="V34" s="58"/>
-      <c r="W34" s="58"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="97"/>
+      <c r="N34" s="97"/>
+      <c r="O34" s="97"/>
+      <c r="P34" s="97"/>
+      <c r="Q34" s="97"/>
+      <c r="R34" s="97"/>
+      <c r="S34" s="97"/>
+      <c r="T34" s="97"/>
+      <c r="U34" s="97"/>
+      <c r="V34" s="97"/>
+      <c r="W34" s="97"/>
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="1:24" s="4" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2584,155 +2584,155 @@
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="130" t="s">
+      <c r="B36" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="131"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="132"/>
-      <c r="F36" s="131" t="s">
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="131"/>
-      <c r="H36" s="131"/>
-      <c r="I36" s="131"/>
-      <c r="J36" s="131"/>
-      <c r="K36" s="131"/>
-      <c r="L36" s="131"/>
-      <c r="M36" s="131"/>
-      <c r="N36" s="138"/>
-      <c r="O36" s="140" t="s">
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="87"/>
+      <c r="O36" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="P36" s="140"/>
-      <c r="Q36" s="140"/>
-      <c r="R36" s="140"/>
-      <c r="S36" s="107" t="s">
+      <c r="P36" s="89"/>
+      <c r="Q36" s="89"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="T36" s="108"/>
-      <c r="U36" s="108"/>
-      <c r="V36" s="109"/>
+      <c r="T36" s="92"/>
+      <c r="U36" s="92"/>
+      <c r="V36" s="93"/>
       <c r="W36" s="23"/>
     </row>
     <row r="37" spans="1:24" s="4" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="133"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="134"/>
-      <c r="E37" s="135"/>
-      <c r="F37" s="134"/>
-      <c r="G37" s="134"/>
-      <c r="H37" s="134"/>
-      <c r="I37" s="134"/>
-      <c r="J37" s="134"/>
-      <c r="K37" s="134"/>
-      <c r="L37" s="134"/>
-      <c r="M37" s="134"/>
-      <c r="N37" s="139"/>
-      <c r="O37" s="141" t="s">
+      <c r="B37" s="84"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="88"/>
+      <c r="O37" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="P37" s="141"/>
-      <c r="Q37" s="141" t="s">
+      <c r="P37" s="90"/>
+      <c r="Q37" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="R37" s="141"/>
-      <c r="S37" s="110"/>
-      <c r="T37" s="111"/>
-      <c r="U37" s="111"/>
-      <c r="V37" s="112"/>
+      <c r="R37" s="90"/>
+      <c r="S37" s="94"/>
+      <c r="T37" s="95"/>
+      <c r="U37" s="95"/>
+      <c r="V37" s="96"/>
       <c r="W37" s="23"/>
     </row>
     <row r="38" spans="1:24" s="4" customFormat="1" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="118" t="s">
+      <c r="B38" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="64"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="61">
+        <v>43158</v>
+      </c>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="61">
+        <v>43158</v>
+      </c>
+      <c r="R38" s="62"/>
+      <c r="S38" s="98"/>
+      <c r="T38" s="99"/>
+      <c r="U38" s="99"/>
+      <c r="V38" s="100"/>
+      <c r="W38" s="23"/>
+    </row>
+    <row r="39" spans="1:24" s="4" customFormat="1" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="136" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="137"/>
-      <c r="H38" s="137"/>
-      <c r="I38" s="137"/>
-      <c r="J38" s="137"/>
-      <c r="K38" s="137"/>
-      <c r="L38" s="137"/>
-      <c r="M38" s="137"/>
-      <c r="N38" s="145"/>
-      <c r="O38" s="113">
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="65"/>
+      <c r="O39" s="61">
         <v>43158</v>
       </c>
-      <c r="P38" s="114"/>
-      <c r="Q38" s="113">
+      <c r="P39" s="62"/>
+      <c r="Q39" s="61">
         <v>43158</v>
       </c>
-      <c r="R38" s="114"/>
-      <c r="S38" s="115"/>
-      <c r="T38" s="116"/>
-      <c r="U38" s="116"/>
-      <c r="V38" s="117"/>
-      <c r="W38" s="23"/>
-    </row>
-    <row r="39" spans="1:24" s="4" customFormat="1" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="118" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="120"/>
-      <c r="F39" s="136" t="s">
+      <c r="R39" s="62"/>
+      <c r="S39" s="98"/>
+      <c r="T39" s="99"/>
+      <c r="U39" s="99"/>
+      <c r="V39" s="100"/>
+      <c r="W39" s="23"/>
+    </row>
+    <row r="40" spans="1:24" s="4" customFormat="1" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="137"/>
-      <c r="H39" s="137"/>
-      <c r="I39" s="137"/>
-      <c r="J39" s="137"/>
-      <c r="K39" s="137"/>
-      <c r="L39" s="137"/>
-      <c r="M39" s="137"/>
-      <c r="N39" s="145"/>
-      <c r="O39" s="113">
-        <v>43158</v>
-      </c>
-      <c r="P39" s="114"/>
-      <c r="Q39" s="113">
-        <v>43158</v>
-      </c>
-      <c r="R39" s="114"/>
-      <c r="S39" s="115"/>
-      <c r="T39" s="116"/>
-      <c r="U39" s="116"/>
-      <c r="V39" s="117"/>
-      <c r="W39" s="23"/>
-    </row>
-    <row r="40" spans="1:24" s="4" customFormat="1" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="118" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="119"/>
-      <c r="D40" s="119"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="136" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="137"/>
-      <c r="H40" s="137"/>
-      <c r="I40" s="137"/>
-      <c r="J40" s="137"/>
-      <c r="K40" s="137"/>
-      <c r="L40" s="137"/>
-      <c r="M40" s="137"/>
-      <c r="N40" s="145"/>
-      <c r="O40" s="113">
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="64"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64"/>
+      <c r="N40" s="65"/>
+      <c r="O40" s="61">
         <v>43164</v>
       </c>
-      <c r="P40" s="114"/>
-      <c r="Q40" s="113">
+      <c r="P40" s="62"/>
+      <c r="Q40" s="61">
         <v>43172</v>
       </c>
-      <c r="R40" s="114"/>
+      <c r="R40" s="62"/>
       <c r="S40" s="55"/>
       <c r="T40" s="56"/>
       <c r="U40" s="56"/>
@@ -2740,31 +2740,31 @@
       <c r="W40" s="23"/>
     </row>
     <row r="41" spans="1:24" s="4" customFormat="1" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="118" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="119"/>
-      <c r="D41" s="119"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="136" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" s="137"/>
-      <c r="H41" s="137"/>
-      <c r="I41" s="137"/>
-      <c r="J41" s="137"/>
-      <c r="K41" s="137"/>
-      <c r="L41" s="137"/>
-      <c r="M41" s="137"/>
-      <c r="N41" s="145"/>
-      <c r="O41" s="113">
+      <c r="B41" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="64"/>
+      <c r="K41" s="64"/>
+      <c r="L41" s="64"/>
+      <c r="M41" s="64"/>
+      <c r="N41" s="65"/>
+      <c r="O41" s="61">
         <v>43164</v>
       </c>
-      <c r="P41" s="114"/>
-      <c r="Q41" s="113">
+      <c r="P41" s="62"/>
+      <c r="Q41" s="61">
         <v>43172</v>
       </c>
-      <c r="R41" s="114"/>
+      <c r="R41" s="62"/>
       <c r="S41" s="55"/>
       <c r="T41" s="56"/>
       <c r="U41" s="56"/>
@@ -2772,67 +2772,67 @@
       <c r="W41" s="23"/>
     </row>
     <row r="42" spans="1:24" s="4" customFormat="1" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="118" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="119"/>
-      <c r="D42" s="119"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="136" t="s">
-        <v>77</v>
-      </c>
-      <c r="G42" s="137"/>
-      <c r="H42" s="137"/>
-      <c r="I42" s="137"/>
-      <c r="J42" s="137"/>
-      <c r="K42" s="137"/>
-      <c r="L42" s="137"/>
-      <c r="M42" s="137"/>
-      <c r="N42" s="145"/>
-      <c r="O42" s="113">
+      <c r="B42" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="64"/>
+      <c r="N42" s="65"/>
+      <c r="O42" s="61">
         <v>43165</v>
       </c>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="113">
+      <c r="P42" s="62"/>
+      <c r="Q42" s="61">
         <v>43166</v>
       </c>
-      <c r="R42" s="114"/>
-      <c r="S42" s="142"/>
-      <c r="T42" s="143"/>
-      <c r="U42" s="143"/>
-      <c r="V42" s="144"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="58"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="59"/>
+      <c r="V42" s="60"/>
       <c r="W42" s="23"/>
     </row>
     <row r="43" spans="1:24" s="4" customFormat="1" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="118" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="136" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" s="137"/>
-      <c r="H43" s="137"/>
-      <c r="I43" s="137"/>
-      <c r="J43" s="137"/>
-      <c r="K43" s="137"/>
-      <c r="L43" s="137"/>
-      <c r="M43" s="137"/>
-      <c r="N43" s="145"/>
-      <c r="O43" s="113">
+      <c r="B43" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64"/>
+      <c r="N43" s="65"/>
+      <c r="O43" s="61">
         <v>43172</v>
       </c>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="113">
+      <c r="P43" s="62"/>
+      <c r="Q43" s="61">
         <v>43172</v>
       </c>
-      <c r="R43" s="114"/>
-      <c r="S43" s="142"/>
-      <c r="T43" s="143"/>
-      <c r="U43" s="143"/>
-      <c r="V43" s="144"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="58"/>
+      <c r="T43" s="59"/>
+      <c r="U43" s="59"/>
+      <c r="V43" s="60"/>
       <c r="W43" s="23"/>
     </row>
     <row r="44" spans="1:24" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2861,30 +2861,30 @@
       <c r="W44" s="31"/>
     </row>
     <row r="45" spans="1:24" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
-      <c r="P45" s="58"/>
-      <c r="Q45" s="58"/>
-      <c r="R45" s="58"/>
-      <c r="S45" s="58"/>
-      <c r="T45" s="58"/>
-      <c r="U45" s="58"/>
-      <c r="V45" s="58"/>
-      <c r="W45" s="58"/>
+      <c r="C45" s="97"/>
+      <c r="D45" s="97"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="97"/>
+      <c r="K45" s="97"/>
+      <c r="L45" s="97"/>
+      <c r="M45" s="97"/>
+      <c r="N45" s="97"/>
+      <c r="O45" s="97"/>
+      <c r="P45" s="97"/>
+      <c r="Q45" s="97"/>
+      <c r="R45" s="97"/>
+      <c r="S45" s="97"/>
+      <c r="T45" s="97"/>
+      <c r="U45" s="97"/>
+      <c r="V45" s="97"/>
+      <c r="W45" s="97"/>
       <c r="X45" s="2"/>
     </row>
     <row r="46" spans="1:24" s="4" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2914,29 +2914,29 @@
       <c r="X46" s="2"/>
     </row>
     <row r="47" spans="1:24" s="4" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="121" t="s">
+      <c r="B47" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="122"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="122"/>
-      <c r="G47" s="122"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="122"/>
-      <c r="J47" s="122"/>
-      <c r="K47" s="122"/>
-      <c r="L47" s="122"/>
-      <c r="M47" s="122"/>
-      <c r="N47" s="122"/>
-      <c r="O47" s="122"/>
-      <c r="P47" s="122"/>
-      <c r="Q47" s="122"/>
-      <c r="R47" s="122"/>
-      <c r="S47" s="122"/>
-      <c r="T47" s="122"/>
-      <c r="U47" s="122"/>
-      <c r="V47" s="123"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="70"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="70"/>
+      <c r="M47" s="70"/>
+      <c r="N47" s="70"/>
+      <c r="O47" s="70"/>
+      <c r="P47" s="70"/>
+      <c r="Q47" s="70"/>
+      <c r="R47" s="70"/>
+      <c r="S47" s="70"/>
+      <c r="T47" s="70"/>
+      <c r="U47" s="70"/>
+      <c r="V47" s="71"/>
       <c r="W47" s="23"/>
     </row>
     <row r="48" spans="1:24" s="4" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3007,20 +3007,52 @@
     <row r="90" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="S42:V42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="F42:N42"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="S43:V43"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:N43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="F40:N40"/>
-    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B34:W34"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="B7:W7"/>
+    <mergeCell ref="D29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="P10:R12"/>
+    <mergeCell ref="E10:O10"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="D1:W1"/>
+    <mergeCell ref="D2:W2"/>
+    <mergeCell ref="D4:W4"/>
+    <mergeCell ref="D3:W3"/>
+    <mergeCell ref="D5:W5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="R29:V29"/>
+    <mergeCell ref="R31:V31"/>
+    <mergeCell ref="E16:O16"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="B22:W22"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="F25:P25"/>
+    <mergeCell ref="R25:V25"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="B45:W45"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="S39:V39"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="S38:V38"/>
+    <mergeCell ref="F41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="B41:E41"/>
     <mergeCell ref="B47:V47"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="J18:L18"/>
@@ -3037,52 +3069,20 @@
     <mergeCell ref="O37:P37"/>
     <mergeCell ref="Q37:R37"/>
     <mergeCell ref="S36:V37"/>
-    <mergeCell ref="B45:W45"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="S39:V39"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="S38:V38"/>
-    <mergeCell ref="F41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="R29:V29"/>
-    <mergeCell ref="R31:V31"/>
-    <mergeCell ref="E16:O16"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="B22:W22"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="F25:P25"/>
-    <mergeCell ref="R25:V25"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="D1:W1"/>
-    <mergeCell ref="D2:W2"/>
-    <mergeCell ref="D4:W4"/>
-    <mergeCell ref="D3:W3"/>
-    <mergeCell ref="D5:W5"/>
-    <mergeCell ref="B34:W34"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="B7:W7"/>
-    <mergeCell ref="D29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:P29"/>
-    <mergeCell ref="P10:R12"/>
-    <mergeCell ref="E10:O10"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="S43:V43"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:N43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="F40:N40"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="S42:V42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="F42:N42"/>
+    <mergeCell ref="B42:E42"/>
   </mergeCells>
   <dataValidations xWindow="662" yWindow="599" count="2">
     <dataValidation type="textLength" errorStyle="information" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Máximo 300 caracteres" error="Excede el número maximo de caracteres" promptTitle="Introducir " prompt="Máximo 300 caracteres" sqref="F38:N38" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>